<commit_message>
Update filament path options .xlsx
</commit_message>
<xml_diff>
--- a/Document Library/filament path options .xlsx
+++ b/Document Library/filament path options .xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="47">
   <si>
     <t xml:space="preserve">Easy to load </t>
   </si>
@@ -145,6 +145,18 @@
   </si>
   <si>
     <t>PTFE tube  may need to be clipped into place after closing drawer, else be waving in the breeze  , loose spot for desicant container</t>
+  </si>
+  <si>
+    <t xml:space="preserve">up througn  base near front </t>
+  </si>
+  <si>
+    <t>1200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exit path out top of printer </t>
+  </si>
+  <si>
+    <t>top of printer</t>
   </si>
 </sst>
 </file>
@@ -198,7 +210,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -221,13 +233,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -237,9 +262,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -278,18 +300,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -303,7 +313,6 @@
     <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -320,6 +329,25 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -744,443 +772,483 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.109375" style="10" customWidth="1"/>
-    <col min="2" max="2" width="38.6640625" style="11" customWidth="1"/>
+    <col min="1" max="1" width="3.109375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" style="10" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.88671875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12.77734375" style="6" customWidth="1"/>
+    <col min="6" max="6" width="12.77734375" style="5" customWidth="1"/>
     <col min="7" max="7" width="11.77734375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5546875" style="7" customWidth="1"/>
-    <col min="9" max="9" width="14.5546875" style="9" customWidth="1"/>
-    <col min="10" max="10" width="38" style="8" customWidth="1"/>
-    <col min="11" max="11" width="8.88671875" style="9"/>
-    <col min="14" max="14" width="10.44140625" customWidth="1"/>
+    <col min="8" max="8" width="14.5546875" style="6" customWidth="1"/>
+    <col min="9" max="9" width="14.5546875" style="8" customWidth="1"/>
+    <col min="10" max="10" width="38" style="7" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" style="8"/>
+    <col min="14" max="14" width="12.77734375" customWidth="1"/>
+    <col min="15" max="15" width="12.21875" customWidth="1"/>
     <col min="16" max="16" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="72" x14ac:dyDescent="0.3">
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="19" t="s">
+      <c r="L1" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="M1" s="19" t="s">
+      <c r="M1" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="N1" s="19" t="s">
+      <c r="N1" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="O1" s="19" t="s">
+      <c r="O1" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="P1" s="19" t="s">
+      <c r="P1" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" s="19" t="s">
+      <c r="Q1" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="R1" s="17"/>
+      <c r="R1" s="33"/>
     </row>
     <row r="2" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="28" t="s">
+      <c r="D2" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="27" t="s">
+      <c r="G2" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="27" t="s">
+      <c r="I2" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="27" t="s">
+      <c r="J2" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="25">
+      <c r="K2" s="20">
         <v>1</v>
       </c>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="25"/>
-      <c r="S2" s="35"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="29"/>
     </row>
     <row r="3" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="28" t="s">
+      <c r="D3" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="25" t="s">
+      <c r="G3" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="J3" s="24"/>
-      <c r="K3" s="25">
+      <c r="I3" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="19"/>
+      <c r="K3" s="20">
         <v>2</v>
       </c>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="25"/>
-      <c r="R3" s="25"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="34"/>
     </row>
     <row r="4" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="E4" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="34" t="s">
+      <c r="F4" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="33" t="s">
+      <c r="G4" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="I4" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="J4" s="33" t="s">
+      <c r="H4" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="31">
+      <c r="K4" s="25">
         <v>3</v>
       </c>
-      <c r="L4" s="31">
+      <c r="L4" s="25">
         <v>100</v>
       </c>
-      <c r="M4" s="31">
+      <c r="M4" s="25">
         <v>3</v>
       </c>
-      <c r="N4" s="31">
-        <v>5</v>
-      </c>
-      <c r="O4" s="31">
-        <v>5</v>
-      </c>
-      <c r="P4" s="31" t="s">
+      <c r="N4" s="25">
+        <v>5</v>
+      </c>
+      <c r="O4" s="25">
+        <v>5</v>
+      </c>
+      <c r="P4" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="Q4" s="31" t="s">
+      <c r="Q4" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="R4" s="31"/>
+      <c r="R4" s="35"/>
     </row>
     <row r="5" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="28" t="s">
+      <c r="D5" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" s="25" t="s">
+      <c r="G5" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="J5" s="27" t="s">
+      <c r="I5" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="K5" s="25">
+      <c r="K5" s="20">
         <v>4</v>
       </c>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="25"/>
-      <c r="O5" s="25"/>
-      <c r="P5" s="25"/>
-      <c r="Q5" s="25"/>
-      <c r="R5" s="25"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="31"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="34"/>
     </row>
     <row r="6" spans="1:19" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="33" t="s">
+      <c r="D6" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="34" t="s">
+      <c r="F6" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="33" t="s">
+      <c r="G6" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="I6" s="31" t="s">
+      <c r="H6" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="33" t="s">
+      <c r="J6" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="K6" s="31">
-        <v>5</v>
-      </c>
-      <c r="L6" s="31">
+      <c r="K6" s="25">
+        <v>5</v>
+      </c>
+      <c r="L6" s="25">
         <v>100</v>
       </c>
-      <c r="M6" s="31">
+      <c r="M6" s="25">
         <v>2</v>
       </c>
-      <c r="N6" s="31">
-        <v>5</v>
-      </c>
-      <c r="O6" s="31">
-        <v>5</v>
-      </c>
-      <c r="P6" s="31" t="s">
+      <c r="N6" s="25">
+        <v>5</v>
+      </c>
+      <c r="O6" s="25">
+        <v>5</v>
+      </c>
+      <c r="P6" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="Q6" s="31" t="s">
+      <c r="Q6" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="R6" s="31"/>
+      <c r="R6" s="35"/>
     </row>
     <row r="7" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="28" t="s">
+      <c r="D7" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="H7" s="25" t="s">
+      <c r="G7" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="J7" s="26" t="s">
+      <c r="I7" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="J7" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="K7" s="25">
+      <c r="K7" s="20">
         <v>4</v>
       </c>
-      <c r="L7" s="25"/>
-      <c r="M7" s="25"/>
-      <c r="N7" s="25"/>
-      <c r="O7" s="25"/>
-      <c r="P7" s="25"/>
-      <c r="Q7" s="25"/>
-      <c r="R7" s="25"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="31"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="34"/>
     </row>
     <row r="8" spans="1:19" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="29"/>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" s="28" t="s">
+      <c r="D8" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="H8" s="25" t="s">
+      <c r="G8" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="J8" s="27" t="s">
+      <c r="I8" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="J8" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="K8" s="25">
+      <c r="K8" s="20">
         <v>6</v>
       </c>
-      <c r="L8" s="25"/>
-      <c r="M8" s="25"/>
-      <c r="N8" s="25"/>
-      <c r="O8" s="25"/>
-      <c r="P8" s="25"/>
-      <c r="Q8" s="25"/>
-      <c r="R8" s="25"/>
-    </row>
-    <row r="9" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="20"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="21"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="31"/>
+      <c r="Q8" s="20"/>
+      <c r="R8" s="34"/>
+    </row>
+    <row r="9" spans="1:19" s="15" customFormat="1" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="J9" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="K9" s="25">
+        <v>2</v>
+      </c>
+      <c r="L9" s="25">
+        <v>60</v>
+      </c>
+      <c r="M9" s="25">
+        <v>4</v>
+      </c>
+      <c r="N9" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="O9" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="P9" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q9" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="R9" s="36"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D10" s="3"/>
-      <c r="F10" s="5"/>
+      <c r="F10" s="4"/>
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="5"/>
+      <c r="F11" s="4"/>
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D12" s="3"/>
-      <c r="F12" s="5"/>
+      <c r="F12" s="4"/>
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="16" t="s">
         <v>33</v>
       </c>
       <c r="D13" s="3"/>
-      <c r="F13" s="5"/>
+      <c r="F13" s="4"/>
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D14" s="3"/>
-      <c r="F14" s="5"/>
+      <c r="F14" s="4"/>
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D15" s="3"/>
-      <c r="F15" s="5"/>
+      <c r="F15" s="4"/>
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D16" s="3"/>
-      <c r="F16" s="5"/>
+      <c r="F16" s="4"/>
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D17" s="3"/>
-      <c r="F17" s="5"/>
+      <c r="F17" s="4"/>
       <c r="G17" s="2"/>
     </row>
     <row r="18" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D18" s="3"/>
-      <c r="F18" s="5"/>
+      <c r="F18" s="4"/>
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D19" s="3"/>
-      <c r="F19" s="5"/>
+      <c r="F19" s="4"/>
       <c r="G19" s="2"/>
     </row>
   </sheetData>

</xml_diff>